<commit_message>
fix: memperbaiki struktur tabel invoice. add: menambahkan api response untuk menampilkan data invoice
</commit_message>
<xml_diff>
--- a/database/data/demoSubCategory.xlsx
+++ b/database/data/demoSubCategory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIN WEB\GIN WEB\project\Koperasi App\koperasi-api\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC46603-A806-453C-8A4C-A0C67150FF9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D1D75C-7B6C-49AC-8DA3-BFBFE2ACC674}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{630C9707-7736-476D-A265-100C96DBDA12}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>type</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>simpanan pokok</t>
+  </si>
+  <si>
+    <t>simpanan wajib khusus</t>
   </si>
 </sst>
 </file>
@@ -445,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5BF2FD-C71F-42B8-9190-1778E4E809B2}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,6 +602,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: response member dan sub kategori untuk invoice
</commit_message>
<xml_diff>
--- a/database/data/demoSubCategory.xlsx
+++ b/database/data/demoSubCategory.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -22,6 +22,9 @@
     <t>category</t>
   </si>
   <si>
+    <t>type payment</t>
+  </si>
+  <si>
     <t>simpanan pokok</t>
   </si>
   <si>
@@ -31,13 +34,22 @@
     <t>simpanan</t>
   </si>
   <si>
+    <t>once</t>
+  </si>
+  <si>
     <t>simpanan wajib</t>
   </si>
   <si>
+    <t>monthly</t>
+  </si>
+  <si>
     <t>simpanan wajib khusus</t>
   </si>
   <si>
     <t>simpanan sukarela</t>
+  </si>
+  <si>
+    <t>anytime</t>
   </si>
   <si>
     <t>tabungan rekreasi</t>
@@ -80,7 +92,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -91,7 +103,16 @@
       <b/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <color theme="1"/>
@@ -119,15 +140,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -347,9 +371,9 @@
     <col customWidth="1" min="1" max="1" width="35.57"/>
     <col customWidth="1" min="2" max="2" width="14.86"/>
     <col customWidth="1" min="3" max="3" width="26.29"/>
-    <col customWidth="1" min="4" max="5" width="8.71"/>
+    <col customWidth="1" min="4" max="4" width="17.71"/>
+    <col customWidth="1" min="5" max="5" width="8.71"/>
     <col customWidth="1" min="6" max="6" width="21.71"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -362,126 +386,162 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
+      <c r="A4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
+      <c r="A5" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
+      <c r="A6" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>